<commit_message>
edit RAM in H370-plus
</commit_message>
<xml_diff>
--- a/fides computers.xlsx
+++ b/fides computers.xlsx
@@ -163,7 +163,7 @@
     <t>INTEL Pentium Gold G5400, BOX</t>
   </si>
   <si>
-    <t>Patriot PVE48G266C6KGY RTL PC4-21300 CL16 DIMM 288-pin 1.2В</t>
+    <t>PATRIOT Viper Elite PVE48G240C5KRD DDR4 - 2x 4Гб 2400</t>
   </si>
 </sst>
 </file>
@@ -405,21 +405,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -429,19 +442,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -783,7 +783,7 @@
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -804,27 +804,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="47"/>
-      <c r="J1" s="45" t="s">
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="40"/>
+      <c r="J1" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="47"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="40"/>
       <c r="S1" s="36"/>
     </row>
     <row r="2" spans="1:19" ht="42" customHeight="1" x14ac:dyDescent="0.25">
@@ -1306,43 +1306,43 @@
       <c r="R11" s="2"/>
     </row>
     <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="42">
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="47">
         <f>SUM(D10,D9,D8,G7,H6,D5,D4,D3)</f>
         <v>38589</v>
       </c>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="44"/>
-      <c r="J12" s="40" t="s">
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="49"/>
+      <c r="J12" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="K12" s="41"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="48">
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="43">
         <f>SUM(N10,N9,N8,N7,M6,N5,N4,M3)</f>
         <v>36385</v>
       </c>
-      <c r="N12" s="38"/>
-      <c r="O12" s="38"/>
-      <c r="P12" s="38"/>
-      <c r="Q12" s="38"/>
-      <c r="R12" s="39"/>
+      <c r="N12" s="44"/>
+      <c r="O12" s="44"/>
+      <c r="P12" s="44"/>
+      <c r="Q12" s="44"/>
+      <c r="R12" s="45"/>
     </row>
     <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J13" s="37" t="s">
+      <c r="J13" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="K13" s="38"/>
-      <c r="L13" s="39"/>
+      <c r="K13" s="44"/>
+      <c r="L13" s="45"/>
     </row>
     <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N15" s="49"/>
+      <c r="N15" s="37"/>
     </row>
     <row r="16" spans="1:19" ht="53.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J16" s="22"/>
@@ -1350,17 +1350,17 @@
       <c r="L16" s="22"/>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="47"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="40"/>
       <c r="J17" s="23"/>
     </row>
     <row r="18" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1488,7 +1488,7 @@
         <v>24</v>
       </c>
       <c r="F22" s="17">
-        <v>7350</v>
+        <v>6940</v>
       </c>
       <c r="G22" s="25" t="s">
         <v>24</v>
@@ -1616,41 +1616,41 @@
       <c r="I27" s="2"/>
     </row>
     <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="40" t="s">
+      <c r="A28" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="41"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="48">
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="43">
         <f>SUM(E23:E26,F22,F21,F20,D19)</f>
-        <v>37928</v>
-      </c>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="39"/>
+        <v>37518</v>
+      </c>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="45"/>
     </row>
     <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="39"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A17:I17"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D28:I28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="J13:L13"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="D12:H12"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="J12:L12"/>
     <mergeCell ref="J1:R1"/>
     <mergeCell ref="M12:R12"/>
+    <mergeCell ref="A17:I17"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D28:I28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="J13:L13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
change MB B250-plus on B250M-A
</commit_message>
<xml_diff>
--- a/fides computers.xlsx
+++ b/fides computers.xlsx
@@ -141,9 +141,6 @@
     <t>ASUS PRIME B250-PLUS</t>
   </si>
   <si>
-    <t>на материнской ASUS PRIME B250-PLUS</t>
-  </si>
-  <si>
     <t xml:space="preserve">Patriot DDR4 DIMM 8GB Kit 2x4Gb PSD48G2133KH
 </t>
   </si>
@@ -164,6 +161,9 @@
   </si>
   <si>
     <t>PATRIOT Viper Elite PVE48G240C5KRD DDR4 - 2x 4Гб 2400</t>
+  </si>
+  <si>
+    <t>на материнской ASUS PRIME B250M-A</t>
   </si>
 </sst>
 </file>
@@ -406,21 +406,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -430,6 +415,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -441,6 +432,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -782,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -804,27 +804,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="45"/>
-      <c r="J1" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44"/>
-      <c r="R1" s="45"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="40"/>
+      <c r="J1" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="40"/>
       <c r="S1" s="36"/>
     </row>
     <row r="2" spans="1:19" ht="42" customHeight="1" x14ac:dyDescent="0.3">
@@ -969,7 +969,7 @@
         <v>6056</v>
       </c>
       <c r="N4" s="7">
-        <v>5590</v>
+        <v>5290</v>
       </c>
       <c r="O4" s="18">
         <v>5650</v>
@@ -1063,7 +1063,7 @@
         <v>9</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M6" s="7">
         <v>6347</v>
@@ -1212,7 +1212,7 @@
         <v>21</v>
       </c>
       <c r="L9" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M9" s="14" t="s">
         <v>24</v>
@@ -1257,7 +1257,7 @@
         <v>15</v>
       </c>
       <c r="L10" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M10" s="18" t="s">
         <v>24</v>
@@ -1306,40 +1306,40 @@
       <c r="R11" s="2"/>
     </row>
     <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="40">
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="47">
         <f>SUM(D10,D9,D8,G7,H6,D5,D4,D3)</f>
         <v>38589</v>
       </c>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="42"/>
-      <c r="J12" s="38" t="s">
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="49"/>
+      <c r="J12" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="K12" s="39"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="46">
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="43">
         <f>SUM(N10,N9,N8,N7,M6,N5,N4,M3)</f>
-        <v>36385</v>
-      </c>
-      <c r="N12" s="47"/>
-      <c r="O12" s="47"/>
-      <c r="P12" s="47"/>
-      <c r="Q12" s="47"/>
-      <c r="R12" s="48"/>
+        <v>36085</v>
+      </c>
+      <c r="N12" s="44"/>
+      <c r="O12" s="44"/>
+      <c r="P12" s="44"/>
+      <c r="Q12" s="44"/>
+      <c r="R12" s="45"/>
     </row>
     <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J13" s="49" t="s">
+      <c r="J13" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="K13" s="47"/>
-      <c r="L13" s="48"/>
+      <c r="K13" s="44"/>
+      <c r="L13" s="45"/>
     </row>
     <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N15" s="37"/>
@@ -1350,17 +1350,17 @@
       <c r="L16" s="22"/>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="45"/>
+      <c r="A17" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="40"/>
       <c r="J17" s="23"/>
     </row>
     <row r="18" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1427,7 +1427,7 @@
         <v>4</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>24</v>
@@ -1454,7 +1454,7 @@
         <v>6</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>24</v>
@@ -1479,7 +1479,7 @@
         <v>9</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>24</v>
@@ -1558,7 +1558,7 @@
         <v>21</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>24</v>
@@ -1583,7 +1583,7 @@
         <v>15</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>24</v>
@@ -1616,41 +1616,41 @@
       <c r="I27" s="2"/>
     </row>
     <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="46">
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="43">
         <f>SUM(E23:E26,F22,F21,F20,D19)</f>
         <v>37518</v>
       </c>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="47"/>
-      <c r="I28" s="48"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="45"/>
     </row>
     <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="49" t="s">
+      <c r="A29" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="47"/>
-      <c r="C29" s="48"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A17:I17"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D28:I28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="J13:L13"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="D12:H12"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="J12:L12"/>
     <mergeCell ref="J1:R1"/>
     <mergeCell ref="M12:R12"/>
+    <mergeCell ref="A17:I17"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D28:I28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="J13:L13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
edit cell with name MB in b250m-a
</commit_message>
<xml_diff>
--- a/fides computers.xlsx
+++ b/fides computers.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mv.savenkov\Desktop\fidesComputers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fazer\Desktop\comps\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="10128"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10125"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -138,9 +138,6 @@
     <t xml:space="preserve"> в компьютер маркет на 450W за 1593  нет в наличии                    </t>
   </si>
   <si>
-    <t>ASUS PRIME B250-PLUS</t>
-  </si>
-  <si>
     <t xml:space="preserve">Patriot DDR4 DIMM 8GB Kit 2x4Gb PSD48G2133KH
 </t>
   </si>
@@ -164,6 +161,9 @@
   </si>
   <si>
     <t>на материнской ASUS PRIME B250M-A</t>
+  </si>
+  <si>
+    <t>ASUS PRIME B250M-A</t>
   </si>
 </sst>
 </file>
@@ -406,6 +406,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -415,12 +430,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -432,15 +441,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -782,52 +782,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" customWidth="1"/>
-    <col min="3" max="3" width="22.44140625" customWidth="1"/>
-    <col min="4" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
-    <col min="10" max="10" width="20.44140625" customWidth="1"/>
-    <col min="11" max="11" width="22.44140625" customWidth="1"/>
-    <col min="12" max="12" width="23.5546875" customWidth="1"/>
-    <col min="13" max="13" width="19.109375" customWidth="1"/>
-    <col min="17" max="17" width="21.109375" customWidth="1"/>
-    <col min="18" max="18" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="4" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" customWidth="1"/>
+    <col min="12" max="12" width="23.5703125" customWidth="1"/>
+    <col min="13" max="13" width="19.140625" customWidth="1"/>
+    <col min="17" max="17" width="21.140625" customWidth="1"/>
+    <col min="18" max="18" width="19.7109375" customWidth="1"/>
     <col min="19" max="19" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:19" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="40"/>
-      <c r="J1" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="40"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="45"/>
+      <c r="J1" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="45"/>
       <c r="S1" s="36"/>
     </row>
-    <row r="2" spans="1:19" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -880,7 +880,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="94.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="94.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>1</v>
       </c>
@@ -931,7 +931,7 @@
       </c>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="1:19" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>2</v>
       </c>
@@ -963,7 +963,7 @@
         <v>4</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="M4" s="18">
         <v>6056</v>
@@ -982,7 +982,7 @@
       </c>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" spans="1:19" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>3</v>
       </c>
@@ -1031,7 +1031,7 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="1:19" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>4</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>9</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M6" s="7">
         <v>6347</v>
@@ -1082,7 +1082,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>5</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>6</v>
       </c>
@@ -1182,7 +1182,7 @@
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
     </row>
-    <row r="9" spans="1:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>7</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>21</v>
       </c>
       <c r="L9" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M9" s="14" t="s">
         <v>24</v>
@@ -1229,7 +1229,7 @@
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
     </row>
-    <row r="10" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>8</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>15</v>
       </c>
       <c r="L10" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M10" s="18" t="s">
         <v>24</v>
@@ -1274,7 +1274,7 @@
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
     </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>9</v>
       </c>
@@ -1305,65 +1305,65 @@
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
     </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="41" t="s">
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="47">
+      <c r="B12" s="39"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="40">
         <f>SUM(D10,D9,D8,G7,H6,D5,D4,D3)</f>
         <v>38589</v>
       </c>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="49"/>
-      <c r="J12" s="41" t="s">
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="42"/>
+      <c r="J12" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="K12" s="42"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="43">
+      <c r="K12" s="39"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="46">
         <f>SUM(N10,N9,N8,N7,M6,N5,N4,M3)</f>
         <v>36085</v>
       </c>
-      <c r="N12" s="44"/>
-      <c r="O12" s="44"/>
-      <c r="P12" s="44"/>
-      <c r="Q12" s="44"/>
-      <c r="R12" s="45"/>
-    </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J13" s="46" t="s">
+      <c r="N12" s="47"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="47"/>
+      <c r="R12" s="48"/>
+    </row>
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J13" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="K13" s="44"/>
-      <c r="L13" s="45"/>
-    </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K13" s="47"/>
+      <c r="L13" s="48"/>
+    </row>
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N15" s="37"/>
     </row>
-    <row r="16" spans="1:19" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="53.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J16" s="22"/>
       <c r="K16" s="22"/>
       <c r="L16" s="22"/>
     </row>
-    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="40"/>
+    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="45"/>
       <c r="J17" s="23"/>
     </row>
-    <row r="18" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
         <v>0</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31">
         <v>1</v>
       </c>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:10" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="31">
         <v>2</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>4</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>24</v>
@@ -1446,7 +1446,7 @@
       </c>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="31">
         <v>3</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>6</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>24</v>
@@ -1471,7 +1471,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:10" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="31">
         <v>4</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>9</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>24</v>
@@ -1498,7 +1498,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="31">
         <v>5</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="31">
         <v>6</v>
       </c>
@@ -1550,7 +1550,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="31">
         <v>7</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>21</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>24</v>
@@ -1575,7 +1575,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="31">
         <v>8</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>15</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>24</v>
@@ -1600,7 +1600,7 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="31">
         <v>9</v>
       </c>
@@ -1615,42 +1615,42 @@
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="41" t="s">
+    <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="42"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="43">
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="46">
         <f>SUM(E23:E26,F22,F21,F20,D19)</f>
         <v>37518</v>
       </c>
-      <c r="E28" s="44"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="45"/>
-    </row>
-    <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="46" t="s">
+      <c r="E28" s="47"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="47"/>
+      <c r="H28" s="47"/>
+      <c r="I28" s="48"/>
+    </row>
+    <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="45"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A17:I17"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D28:I28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="J13:L13"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="D12:H12"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="J12:L12"/>
     <mergeCell ref="J1:R1"/>
     <mergeCell ref="M12:R12"/>
-    <mergeCell ref="A17:I17"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D28:I28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="J13:L13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -1665,13 +1665,13 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
-    <col min="3" max="3" width="26.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="26">
         <v>1</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="26">
         <v>2</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="26">
         <v>3</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="26">
         <v>4</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="26">
         <v>5</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="26">
         <v>6</v>
       </c>

</xml_diff>